<commit_message>
ora salvataggio delle tabelle ripulite è effettivo - provato con access
</commit_message>
<xml_diff>
--- a/static/saved_dataframes/tabelle_entita_e_relazionali/is_Acronimo_of.xlsx
+++ b/static/saved_dataframes/tabelle_entita_e_relazionali/is_Acronimo_of.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E250"/>
+  <dimension ref="A1:E247"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -736,12 +736,12 @@
         <v>2000001</v>
       </c>
       <c r="C22" t="n">
-        <v>1000020</v>
+        <v>1000022</v>
       </c>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Ambiente</t>
+          <t>Amianto</t>
         </is>
       </c>
     </row>
@@ -753,12 +753,12 @@
         <v>2000001</v>
       </c>
       <c r="C23" t="n">
-        <v>1000022</v>
+        <v>1000023</v>
       </c>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Amianto</t>
+          <t>Analisi Ambientale</t>
         </is>
       </c>
     </row>
@@ -770,12 +770,12 @@
         <v>2000001</v>
       </c>
       <c r="C24" t="n">
-        <v>1000023</v>
+        <v>1000024</v>
       </c>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Analisi Ambientale</t>
+          <t>Analisi Ambientale Preliminare</t>
         </is>
       </c>
     </row>
@@ -787,12 +787,12 @@
         <v>2000001</v>
       </c>
       <c r="C25" t="n">
-        <v>1000024</v>
+        <v>1000025</v>
       </c>
       <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Analisi Ambientale Preliminare</t>
+          <t>Analisi Costi Benefici Ambientale</t>
         </is>
       </c>
     </row>
@@ -804,12 +804,12 @@
         <v>2000001</v>
       </c>
       <c r="C26" t="n">
-        <v>1000025</v>
+        <v>1000026</v>
       </c>
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Analisi Costi Benefici Ambientale</t>
+          <t>Life Cycle Analysis</t>
         </is>
       </c>
     </row>
@@ -821,12 +821,12 @@
         <v>2000001</v>
       </c>
       <c r="C27" t="n">
-        <v>1000026</v>
+        <v>1000027</v>
       </c>
       <c r="D27" t="inlineStr"/>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Life Cycle Analysis</t>
+          <t>Material Intensità Analysis</t>
         </is>
       </c>
     </row>
@@ -838,12 +838,12 @@
         <v>2000001</v>
       </c>
       <c r="C28" t="n">
-        <v>1000027</v>
+        <v>1000028</v>
       </c>
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Material Intensità Analysis</t>
+          <t>Analisi Multicriteria</t>
         </is>
       </c>
     </row>
@@ -855,12 +855,12 @@
         <v>2000001</v>
       </c>
       <c r="C29" t="n">
-        <v>1000028</v>
+        <v>1000029</v>
       </c>
       <c r="D29" t="inlineStr"/>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Analisi Multicriteria</t>
+          <t>Swot Analysis</t>
         </is>
       </c>
     </row>
@@ -872,12 +872,12 @@
         <v>2000001</v>
       </c>
       <c r="C30" t="n">
-        <v>1000029</v>
+        <v>1000030</v>
       </c>
       <c r="D30" t="inlineStr"/>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Swot Analysis</t>
+          <t>Anidride Solforosa</t>
         </is>
       </c>
     </row>
@@ -889,12 +889,12 @@
         <v>2000001</v>
       </c>
       <c r="C31" t="n">
-        <v>1000030</v>
+        <v>1000031</v>
       </c>
       <c r="D31" t="inlineStr"/>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Anidride Solforosa</t>
+          <t>Antropizzazione</t>
         </is>
       </c>
     </row>
@@ -906,12 +906,12 @@
         <v>2000001</v>
       </c>
       <c r="C32" t="n">
-        <v>1000031</v>
+        <v>1000032</v>
       </c>
       <c r="D32" t="inlineStr"/>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Antropizzazione</t>
+          <t>Approccio Basato Sugli Ecosistemi</t>
         </is>
       </c>
     </row>
@@ -923,12 +923,12 @@
         <v>2000001</v>
       </c>
       <c r="C33" t="n">
-        <v>1000032</v>
+        <v>1000033</v>
       </c>
       <c r="D33" t="inlineStr"/>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Approccio Basato Sugli Ecosistemi</t>
+          <t>Approccio Integrato</t>
         </is>
       </c>
     </row>
@@ -940,12 +940,12 @@
         <v>2000001</v>
       </c>
       <c r="C34" t="n">
-        <v>1000033</v>
+        <v>1000034</v>
       </c>
       <c r="D34" t="inlineStr"/>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Approccio Integrato</t>
+          <t>Aree Protette</t>
         </is>
       </c>
     </row>
@@ -957,12 +957,12 @@
         <v>2000001</v>
       </c>
       <c r="C35" t="n">
-        <v>1000034</v>
+        <v>1000035</v>
       </c>
       <c r="D35" t="inlineStr"/>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Aree Protette</t>
+          <t>Aree Sensibili</t>
         </is>
       </c>
     </row>
@@ -974,12 +974,12 @@
         <v>2000001</v>
       </c>
       <c r="C36" t="n">
-        <v>1000035</v>
+        <v>1000036</v>
       </c>
       <c r="D36" t="inlineStr"/>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Aree Sensibili</t>
+          <t>Aria , Livello Di Qualità Dell'</t>
         </is>
       </c>
     </row>
@@ -991,12 +991,12 @@
         <v>2000001</v>
       </c>
       <c r="C37" t="n">
-        <v>1000036</v>
+        <v>1000037</v>
       </c>
       <c r="D37" t="inlineStr"/>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Aria , Livello Di Qualità Dell'</t>
+          <t>Aspetto Ambientale</t>
         </is>
       </c>
     </row>
@@ -1008,12 +1008,12 @@
         <v>2000001</v>
       </c>
       <c r="C38" t="n">
-        <v>1000037</v>
+        <v>1000038</v>
       </c>
       <c r="D38" t="inlineStr"/>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Aspetto Ambientale</t>
+          <t>Attori</t>
         </is>
       </c>
     </row>
@@ -1025,12 +1025,12 @@
         <v>2000001</v>
       </c>
       <c r="C39" t="n">
-        <v>1000038</v>
+        <v>1000039</v>
       </c>
       <c r="D39" t="inlineStr"/>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Attori</t>
+          <t>Attori Locali</t>
         </is>
       </c>
     </row>
@@ -1042,12 +1042,12 @@
         <v>2000001</v>
       </c>
       <c r="C40" t="n">
-        <v>1000039</v>
+        <v>1000040</v>
       </c>
       <c r="D40" t="inlineStr"/>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Attori Locali</t>
+          <t>Audit Ambientale</t>
         </is>
       </c>
     </row>
@@ -1059,12 +1059,12 @@
         <v>2000001</v>
       </c>
       <c r="C41" t="n">
-        <v>1000040</v>
+        <v>1000041</v>
       </c>
       <c r="D41" t="inlineStr"/>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Audit Ambientale</t>
+          <t>Backcasting</t>
         </is>
       </c>
     </row>
@@ -1076,12 +1076,12 @@
         <v>2000001</v>
       </c>
       <c r="C42" t="n">
-        <v>1000041</v>
+        <v>1000042</v>
       </c>
       <c r="D42" t="inlineStr"/>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Backcasting</t>
+          <t>Baseline Ambientale</t>
         </is>
       </c>
     </row>
@@ -1093,12 +1093,12 @@
         <v>2000001</v>
       </c>
       <c r="C43" t="n">
-        <v>1000042</v>
+        <v>1000043</v>
       </c>
       <c r="D43" t="inlineStr"/>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Baseline Ambientale</t>
+          <t>Benchmark</t>
         </is>
       </c>
     </row>
@@ -1110,12 +1110,12 @@
         <v>2000001</v>
       </c>
       <c r="C44" t="n">
-        <v>1000043</v>
+        <v>1000044</v>
       </c>
       <c r="D44" t="inlineStr"/>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Benchmark</t>
+          <t>Benchmarking Ambientale</t>
         </is>
       </c>
     </row>
@@ -1127,12 +1127,12 @@
         <v>2000001</v>
       </c>
       <c r="C45" t="n">
-        <v>1000044</v>
+        <v>1000045</v>
       </c>
       <c r="D45" t="inlineStr"/>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Benchmarking Ambientale</t>
+          <t>Benessere Degli Animali</t>
         </is>
       </c>
     </row>
@@ -1144,12 +1144,12 @@
         <v>2000001</v>
       </c>
       <c r="C46" t="n">
-        <v>1000045</v>
+        <v>1000046</v>
       </c>
       <c r="D46" t="inlineStr"/>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Benessere Degli Animali</t>
+          <t>Global Commons</t>
         </is>
       </c>
     </row>
@@ -1161,12 +1161,12 @@
         <v>2000001</v>
       </c>
       <c r="C47" t="n">
-        <v>1000046</v>
+        <v>1000047</v>
       </c>
       <c r="D47" t="inlineStr"/>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Global Commons</t>
+          <t>Best Available Technology Not Entailing Excessive Costs</t>
         </is>
       </c>
     </row>
@@ -1178,12 +1178,12 @@
         <v>2000001</v>
       </c>
       <c r="C48" t="n">
-        <v>1000047</v>
+        <v>1000048</v>
       </c>
       <c r="D48" t="inlineStr"/>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Best Available Technology Not Entailing Excessive Costs</t>
+          <t>Best Practicies</t>
         </is>
       </c>
     </row>
@@ -1195,12 +1195,12 @@
         <v>2000001</v>
       </c>
       <c r="C49" t="n">
-        <v>1000048</v>
+        <v>1000049</v>
       </c>
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Best Practicies</t>
+          <t>Bilanci Satellite</t>
         </is>
       </c>
     </row>
@@ -1212,12 +1212,12 @@
         <v>2000001</v>
       </c>
       <c r="C50" t="n">
-        <v>1000049</v>
+        <v>1000050</v>
       </c>
       <c r="D50" t="inlineStr"/>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Bilanci Satellite</t>
+          <t>Bilancio Ambientale</t>
         </is>
       </c>
     </row>
@@ -1229,12 +1229,12 @@
         <v>2000001</v>
       </c>
       <c r="C51" t="n">
-        <v>1000050</v>
+        <v>1000051</v>
       </c>
       <c r="D51" t="inlineStr"/>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Bilancio Ambientale</t>
+          <t>Bilancio Ecologico</t>
         </is>
       </c>
     </row>
@@ -1246,12 +1246,12 @@
         <v>2000001</v>
       </c>
       <c r="C52" t="n">
-        <v>1000051</v>
+        <v>1000052</v>
       </c>
       <c r="D52" t="inlineStr"/>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Bilancio Ecologico</t>
+          <t>Bilancio Ecologico Territoriale</t>
         </is>
       </c>
     </row>
@@ -1263,12 +1263,12 @@
         <v>2000001</v>
       </c>
       <c r="C53" t="n">
-        <v>1000052</v>
+        <v>1000053</v>
       </c>
       <c r="D53" t="inlineStr"/>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Bilancio Ecologico Territoriale</t>
+          <t>Bilancio Partecipativo</t>
         </is>
       </c>
     </row>
@@ -1280,12 +1280,12 @@
         <v>2000001</v>
       </c>
       <c r="C54" t="n">
-        <v>1000052</v>
+        <v>1000054</v>
       </c>
       <c r="D54" t="inlineStr"/>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Bilancio Ecologico Territoriale</t>
+          <t>Bilancio Energetico</t>
         </is>
       </c>
     </row>
@@ -1297,12 +1297,12 @@
         <v>2000001</v>
       </c>
       <c r="C55" t="n">
-        <v>1000054</v>
+        <v>1000055</v>
       </c>
       <c r="D55" t="inlineStr"/>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Bilancio Energetico</t>
+          <t>Bilancio O Rapporto Ambientale</t>
         </is>
       </c>
     </row>
@@ -1314,12 +1314,12 @@
         <v>2000001</v>
       </c>
       <c r="C56" t="n">
-        <v>1000055</v>
+        <v>1000056</v>
       </c>
       <c r="D56" t="inlineStr"/>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Bilancio O Rapporto Ambientale</t>
+          <t>Bioarchitettura E Bioedilizia</t>
         </is>
       </c>
     </row>
@@ -1331,12 +1331,12 @@
         <v>2000001</v>
       </c>
       <c r="C57" t="n">
-        <v>1000053</v>
+        <v>1000057</v>
       </c>
       <c r="D57" t="inlineStr"/>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Bilancio Partecipativo</t>
+          <t>Biodiversità</t>
         </is>
       </c>
     </row>
@@ -1348,12 +1348,12 @@
         <v>2000001</v>
       </c>
       <c r="C58" t="n">
-        <v>1000056</v>
+        <v>1000058</v>
       </c>
       <c r="D58" t="inlineStr"/>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Bioarchitettura E Bioedilizia</t>
+          <t>Biofuels</t>
         </is>
       </c>
     </row>
@@ -1365,12 +1365,12 @@
         <v>2000001</v>
       </c>
       <c r="C59" t="n">
-        <v>1000058</v>
+        <v>1000059</v>
       </c>
       <c r="D59" t="inlineStr"/>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Biofuels</t>
+          <t>Biocenosi</t>
         </is>
       </c>
     </row>
@@ -1382,12 +1382,12 @@
         <v>2000001</v>
       </c>
       <c r="C60" t="n">
-        <v>1000059</v>
+        <v>1000060</v>
       </c>
       <c r="D60" t="inlineStr"/>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Biocenosi</t>
+          <t>Biodegradabile</t>
         </is>
       </c>
     </row>
@@ -1399,12 +1399,12 @@
         <v>2000001</v>
       </c>
       <c r="C61" t="n">
-        <v>1000060</v>
+        <v>1000061</v>
       </c>
       <c r="D61" t="inlineStr"/>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Biodegradabile</t>
+          <t>Bioenergia</t>
         </is>
       </c>
     </row>
@@ -1416,12 +1416,12 @@
         <v>2000001</v>
       </c>
       <c r="C62" t="n">
-        <v>1000057</v>
+        <v>1000062</v>
       </c>
       <c r="D62" t="inlineStr"/>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Biodiversità</t>
+          <t>Biogas</t>
         </is>
       </c>
     </row>
@@ -1433,12 +1433,12 @@
         <v>2000001</v>
       </c>
       <c r="C63" t="n">
-        <v>1000061</v>
+        <v>1000063</v>
       </c>
       <c r="D63" t="inlineStr"/>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Bioenergia</t>
+          <t>Bioetica</t>
         </is>
       </c>
     </row>
@@ -1450,12 +1450,12 @@
         <v>2000001</v>
       </c>
       <c r="C64" t="n">
-        <v>1000063</v>
+        <v>1000064</v>
       </c>
       <c r="D64" t="inlineStr"/>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Bioetica</t>
+          <t>Biofitodepurazione</t>
         </is>
       </c>
     </row>
@@ -1467,12 +1467,12 @@
         <v>2000001</v>
       </c>
       <c r="C65" t="n">
-        <v>1000064</v>
+        <v>1000065</v>
       </c>
       <c r="D65" t="inlineStr"/>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Biofitodepurazione</t>
+          <t>Bioindicatore</t>
         </is>
       </c>
     </row>
@@ -1484,12 +1484,12 @@
         <v>2000001</v>
       </c>
       <c r="C66" t="n">
-        <v>1000062</v>
+        <v>1000066</v>
       </c>
       <c r="D66" t="inlineStr"/>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Biogas</t>
+          <t>Biological Oxygen Demand</t>
         </is>
       </c>
     </row>
@@ -1501,12 +1501,12 @@
         <v>2000001</v>
       </c>
       <c r="C67" t="n">
-        <v>1000065</v>
+        <v>1000067</v>
       </c>
       <c r="D67" t="inlineStr"/>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Bioindicatore</t>
+          <t>Bioingegneria</t>
         </is>
       </c>
     </row>
@@ -1518,12 +1518,12 @@
         <v>2000001</v>
       </c>
       <c r="C68" t="n">
-        <v>1000067</v>
+        <v>1000068</v>
       </c>
       <c r="D68" t="inlineStr"/>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Bioingegneria</t>
+          <t>Bioitaly</t>
         </is>
       </c>
     </row>
@@ -1535,12 +1535,12 @@
         <v>2000001</v>
       </c>
       <c r="C69" t="n">
-        <v>1000068</v>
+        <v>1000069</v>
       </c>
       <c r="D69" t="inlineStr"/>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Bioitaly</t>
+          <t>Bioma</t>
         </is>
       </c>
     </row>
@@ -1552,12 +1552,12 @@
         <v>2000001</v>
       </c>
       <c r="C70" t="n">
-        <v>1000066</v>
+        <v>1000070</v>
       </c>
       <c r="D70" t="inlineStr"/>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Biological Oxygen Demand</t>
+          <t>Biorisanamento</t>
         </is>
       </c>
     </row>
@@ -1569,12 +1569,12 @@
         <v>2000001</v>
       </c>
       <c r="C71" t="n">
-        <v>1000069</v>
+        <v>1000071</v>
       </c>
       <c r="D71" t="inlineStr"/>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Bioma</t>
+          <t>Biomassa</t>
         </is>
       </c>
     </row>
@@ -1586,12 +1586,12 @@
         <v>2000001</v>
       </c>
       <c r="C72" t="n">
-        <v>1000071</v>
+        <v>1000072</v>
       </c>
       <c r="D72" t="inlineStr"/>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Biomassa</t>
+          <t>Biomonitoraggio</t>
         </is>
       </c>
     </row>
@@ -1603,12 +1603,12 @@
         <v>2000001</v>
       </c>
       <c r="C73" t="n">
-        <v>1000072</v>
+        <v>1000073</v>
       </c>
       <c r="D73" t="inlineStr"/>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Biomonitoraggio</t>
+          <t>Biosensori</t>
         </is>
       </c>
     </row>
@@ -1620,12 +1620,12 @@
         <v>2000001</v>
       </c>
       <c r="C74" t="n">
-        <v>1000070</v>
+        <v>1000074</v>
       </c>
       <c r="D74" t="inlineStr"/>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Biorisanamento</t>
+          <t>Biotecnologie</t>
         </is>
       </c>
     </row>
@@ -1637,12 +1637,12 @@
         <v>2000001</v>
       </c>
       <c r="C75" t="n">
-        <v>1000073</v>
+        <v>1000075</v>
       </c>
       <c r="D75" t="inlineStr"/>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Biosensori</t>
+          <t>Biosfera</t>
         </is>
       </c>
     </row>
@@ -1654,12 +1654,12 @@
         <v>2000001</v>
       </c>
       <c r="C76" t="n">
-        <v>1000075</v>
+        <v>1000076</v>
       </c>
       <c r="D76" t="inlineStr"/>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Biosfera</t>
+          <t>Biossido Di Carbonio</t>
         </is>
       </c>
     </row>
@@ -1671,12 +1671,12 @@
         <v>2000001</v>
       </c>
       <c r="C77" t="n">
-        <v>1000076</v>
+        <v>1000077</v>
       </c>
       <c r="D77" t="inlineStr"/>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Biossido Di Carbonio</t>
+          <t>Biotopo</t>
         </is>
       </c>
     </row>
@@ -1688,12 +1688,12 @@
         <v>2000001</v>
       </c>
       <c r="C78" t="n">
-        <v>1000074</v>
+        <v>1000078</v>
       </c>
       <c r="D78" t="inlineStr"/>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Biotecnologie</t>
+          <t>Bottom-Up</t>
         </is>
       </c>
     </row>
@@ -1705,12 +1705,12 @@
         <v>2000001</v>
       </c>
       <c r="C79" t="n">
-        <v>1000077</v>
+        <v>1000079</v>
       </c>
       <c r="D79" t="inlineStr"/>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Biotopo</t>
+          <t>Blueprint For Survival</t>
         </is>
       </c>
     </row>
@@ -1722,12 +1722,12 @@
         <v>2000001</v>
       </c>
       <c r="C80" t="n">
-        <v>1000079</v>
+        <v>1000080</v>
       </c>
       <c r="D80" t="inlineStr"/>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Blueprint For Survival</t>
+          <t>Bonifica</t>
         </is>
       </c>
     </row>
@@ -1739,12 +1739,12 @@
         <v>2000001</v>
       </c>
       <c r="C81" t="n">
-        <v>1000080</v>
+        <v>1000081</v>
       </c>
       <c r="D81" t="inlineStr"/>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Bonifica</t>
+          <t>Cambiamenti Climatici</t>
         </is>
       </c>
     </row>
@@ -1756,12 +1756,12 @@
         <v>2000001</v>
       </c>
       <c r="C82" t="n">
-        <v>1000078</v>
+        <v>1000082</v>
       </c>
       <c r="D82" t="inlineStr"/>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Bottom-Up</t>
+          <t>Caos</t>
         </is>
       </c>
     </row>
@@ -1773,12 +1773,12 @@
         <v>2000001</v>
       </c>
       <c r="C83" t="n">
-        <v>1000081</v>
+        <v>1000083</v>
       </c>
       <c r="D83" t="inlineStr"/>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Cambiamenti Climatici</t>
+          <t>Cambiamento</t>
         </is>
       </c>
     </row>
@@ -1790,12 +1790,12 @@
         <v>2000001</v>
       </c>
       <c r="C84" t="n">
-        <v>1000083</v>
+        <v>1000084</v>
       </c>
       <c r="D84" t="inlineStr"/>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Cambiamento</t>
+          <t>Cambiamento Paradigmatico</t>
         </is>
       </c>
     </row>
@@ -1807,12 +1807,12 @@
         <v>2000001</v>
       </c>
       <c r="C85" t="n">
-        <v>1000084</v>
+        <v>1000085</v>
       </c>
       <c r="D85" t="inlineStr"/>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Cambiamento Paradigmatico</t>
+          <t>Capacity Building</t>
         </is>
       </c>
     </row>
@@ -1824,12 +1824,12 @@
         <v>2000001</v>
       </c>
       <c r="C86" t="n">
-        <v>1000082</v>
+        <v>1000086</v>
       </c>
       <c r="D86" t="inlineStr"/>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Caos</t>
+          <t>Environmental Carrying Capacity</t>
         </is>
       </c>
     </row>
@@ -1841,12 +1841,12 @@
         <v>2000001</v>
       </c>
       <c r="C87" t="n">
-        <v>1000086</v>
+        <v>1000087</v>
       </c>
       <c r="D87" t="inlineStr"/>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Environmental Carrying Capacity</t>
+          <t>Capacità Portante O Capacità Di Carico</t>
         </is>
       </c>
     </row>
@@ -1858,12 +1858,12 @@
         <v>2000001</v>
       </c>
       <c r="C88" t="n">
-        <v>1000087</v>
+        <v>1000088</v>
       </c>
       <c r="D88" t="inlineStr"/>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Capacità Portante O Capacità Di Carico</t>
+          <t>Capitale Naturale</t>
         </is>
       </c>
     </row>
@@ -1875,12 +1875,12 @@
         <v>2000001</v>
       </c>
       <c r="C89" t="n">
-        <v>1000088</v>
+        <v>1000089</v>
       </c>
       <c r="D89" t="inlineStr"/>
       <c r="E89" t="inlineStr">
         <is>
-          <t>Capitale Naturale</t>
+          <t>Capitale Umano</t>
         </is>
       </c>
     </row>
@@ -1892,12 +1892,12 @@
         <v>2000001</v>
       </c>
       <c r="C90" t="n">
-        <v>1000089</v>
+        <v>1000090</v>
       </c>
       <c r="D90" t="inlineStr"/>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Capitale Umano</t>
+          <t>Carbon Tax</t>
         </is>
       </c>
     </row>
@@ -1909,12 +1909,12 @@
         <v>2000001</v>
       </c>
       <c r="C91" t="n">
-        <v>1000090</v>
+        <v>1000091</v>
       </c>
       <c r="D91" t="inlineStr"/>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Carbon Tax</t>
+          <t>Carico Ambientale</t>
         </is>
       </c>
     </row>
@@ -1926,12 +1926,12 @@
         <v>2000001</v>
       </c>
       <c r="C92" t="n">
-        <v>1000091</v>
+        <v>1000092</v>
       </c>
       <c r="D92" t="inlineStr"/>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Carico Ambientale</t>
+          <t>Car-Pool</t>
         </is>
       </c>
     </row>
@@ -1943,12 +1943,12 @@
         <v>2000001</v>
       </c>
       <c r="C93" t="n">
-        <v>1000092</v>
+        <v>1000093</v>
       </c>
       <c r="D93" t="inlineStr"/>
       <c r="E93" t="inlineStr">
         <is>
-          <t>Car-Pool</t>
+          <t>Car-Sharing</t>
         </is>
       </c>
     </row>
@@ -1960,12 +1960,12 @@
         <v>2000001</v>
       </c>
       <c r="C94" t="n">
-        <v>1000093</v>
+        <v>1000094</v>
       </c>
       <c r="D94" t="inlineStr"/>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Car-Sharing</t>
+          <t>Carta Del Turismo Sostenibile</t>
         </is>
       </c>
     </row>
@@ -1977,12 +1977,12 @@
         <v>2000001</v>
       </c>
       <c r="C95" t="n">
-        <v>1000094</v>
+        <v>1000095</v>
       </c>
       <c r="D95" t="inlineStr"/>
       <c r="E95" t="inlineStr">
         <is>
-          <t>Carta Del Turismo Sostenibile</t>
+          <t>Carta Di Aalborg</t>
         </is>
       </c>
     </row>
@@ -1994,12 +1994,12 @@
         <v>2000001</v>
       </c>
       <c r="C96" t="n">
-        <v>1000095</v>
+        <v>1000096</v>
       </c>
       <c r="D96" t="inlineStr"/>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Carta Di Aalborg</t>
+          <t>Carta Sociale</t>
         </is>
       </c>
     </row>
@@ -2011,12 +2011,12 @@
         <v>2000001</v>
       </c>
       <c r="C97" t="n">
-        <v>1000096</v>
+        <v>1000097</v>
       </c>
       <c r="D97" t="inlineStr"/>
       <c r="E97" t="inlineStr">
         <is>
-          <t>Carta Sociale</t>
+          <t>Carte Di Valutazione Della Fragilità, Dissesto E Degrado Ambientale</t>
         </is>
       </c>
     </row>
@@ -2028,12 +2028,12 @@
         <v>2000001</v>
       </c>
       <c r="C98" t="n">
-        <v>1000097</v>
+        <v>1000098</v>
       </c>
       <c r="D98" t="inlineStr"/>
       <c r="E98" t="inlineStr">
         <is>
-          <t>Carte Di Valutazione Della Fragilità, Dissesto E Degrado Ambientale</t>
+          <t>Carte Ecologiche</t>
         </is>
       </c>
     </row>
@@ -2045,12 +2045,12 @@
         <v>2000001</v>
       </c>
       <c r="C99" t="n">
-        <v>1000098</v>
+        <v>1000099</v>
       </c>
       <c r="D99" t="inlineStr"/>
       <c r="E99" t="inlineStr">
         <is>
-          <t>Carte Ecologiche</t>
+          <t>Cartografia</t>
         </is>
       </c>
     </row>
@@ -2062,12 +2062,12 @@
         <v>2000001</v>
       </c>
       <c r="C100" t="n">
-        <v>1000099</v>
+        <v>1000100</v>
       </c>
       <c r="D100" t="inlineStr"/>
       <c r="E100" t="inlineStr">
         <is>
-          <t>Cartografia</t>
+          <t>Centrale Idroelettrica</t>
         </is>
       </c>
     </row>
@@ -2079,12 +2079,12 @@
         <v>2000001</v>
       </c>
       <c r="C101" t="n">
-        <v>1000100</v>
+        <v>1000101</v>
       </c>
       <c r="D101" t="inlineStr"/>
       <c r="E101" t="inlineStr">
         <is>
-          <t>Centrale Idroelettrica</t>
+          <t>Centrale Nucleare</t>
         </is>
       </c>
     </row>
@@ -2096,12 +2096,12 @@
         <v>2000001</v>
       </c>
       <c r="C102" t="n">
-        <v>1000101</v>
+        <v>1000102</v>
       </c>
       <c r="D102" t="inlineStr"/>
       <c r="E102" t="inlineStr">
         <is>
-          <t>Centrale Nucleare</t>
+          <t>Centrale Solare Termoelettrica</t>
         </is>
       </c>
     </row>
@@ -2113,12 +2113,12 @@
         <v>2000001</v>
       </c>
       <c r="C103" t="n">
-        <v>1000102</v>
+        <v>1000103</v>
       </c>
       <c r="D103" t="inlineStr"/>
       <c r="E103" t="inlineStr">
         <is>
-          <t>Centrale Solare Termoelettrica</t>
+          <t>Centrale Termoelettrica</t>
         </is>
       </c>
     </row>
@@ -2130,12 +2130,12 @@
         <v>2000001</v>
       </c>
       <c r="C104" t="n">
-        <v>1000103</v>
+        <v>1000104</v>
       </c>
       <c r="D104" t="inlineStr"/>
       <c r="E104" t="inlineStr">
         <is>
-          <t>Centrale Termoelettrica</t>
+          <t>Certificati Verdi</t>
         </is>
       </c>
     </row>
@@ -2147,12 +2147,12 @@
         <v>2000001</v>
       </c>
       <c r="C105" t="n">
-        <v>1000104</v>
+        <v>1000105</v>
       </c>
       <c r="D105" t="inlineStr"/>
       <c r="E105" t="inlineStr">
         <is>
-          <t>Certificati Verdi</t>
+          <t>Certificazione Ambientale</t>
         </is>
       </c>
     </row>
@@ -2164,12 +2164,12 @@
         <v>2000001</v>
       </c>
       <c r="C106" t="n">
-        <v>1000105</v>
+        <v>1000106</v>
       </c>
       <c r="D106" t="inlineStr"/>
       <c r="E106" t="inlineStr">
         <is>
-          <t>Certificazione Ambientale</t>
+          <t>Check List</t>
         </is>
       </c>
     </row>
@@ -2181,12 +2181,12 @@
         <v>2000001</v>
       </c>
       <c r="C107" t="n">
-        <v>1000106</v>
+        <v>1000107</v>
       </c>
       <c r="D107" t="inlineStr"/>
       <c r="E107" t="inlineStr">
         <is>
-          <t>Check List</t>
+          <t>Chiusura Opposta Ad Apertura</t>
         </is>
       </c>
     </row>
@@ -2198,12 +2198,12 @@
         <v>2000001</v>
       </c>
       <c r="C108" t="n">
-        <v>1000107</v>
+        <v>1000108</v>
       </c>
       <c r="D108" t="inlineStr"/>
       <c r="E108" t="inlineStr">
         <is>
-          <t>Chiusura Opposta Ad Apertura</t>
+          <t>Ciclo</t>
         </is>
       </c>
     </row>
@@ -2215,12 +2215,12 @@
         <v>2000001</v>
       </c>
       <c r="C109" t="n">
-        <v>1000108</v>
+        <v>1000109</v>
       </c>
       <c r="D109" t="inlineStr"/>
       <c r="E109" t="inlineStr">
         <is>
-          <t>Ciclo</t>
+          <t>Ciclo Biologico</t>
         </is>
       </c>
     </row>
@@ -2232,12 +2232,12 @@
         <v>2000001</v>
       </c>
       <c r="C110" t="n">
-        <v>1000109</v>
+        <v>1000110</v>
       </c>
       <c r="D110" t="inlineStr"/>
       <c r="E110" t="inlineStr">
         <is>
-          <t>Ciclo Biologico</t>
+          <t>Ciclo Di Vita</t>
         </is>
       </c>
     </row>
@@ -2249,12 +2249,12 @@
         <v>2000001</v>
       </c>
       <c r="C111" t="n">
-        <v>1000110</v>
+        <v>1000111</v>
       </c>
       <c r="D111" t="inlineStr"/>
       <c r="E111" t="inlineStr">
         <is>
-          <t>Ciclo Di Vita</t>
+          <t>Clean Development Mechanism</t>
         </is>
       </c>
     </row>
@@ -2266,12 +2266,12 @@
         <v>2000001</v>
       </c>
       <c r="C112" t="n">
-        <v>1000111</v>
+        <v>1000112</v>
       </c>
       <c r="D112" t="inlineStr"/>
       <c r="E112" t="inlineStr">
         <is>
-          <t>Clean Development Mechanism</t>
+          <t>Cleaner Production</t>
         </is>
       </c>
     </row>
@@ -2283,12 +2283,12 @@
         <v>2000001</v>
       </c>
       <c r="C113" t="n">
-        <v>1000112</v>
+        <v>1000113</v>
       </c>
       <c r="D113" t="inlineStr"/>
       <c r="E113" t="inlineStr">
         <is>
-          <t>Cleaner Production</t>
+          <t>Clima</t>
         </is>
       </c>
     </row>
@@ -2300,12 +2300,12 @@
         <v>2000001</v>
       </c>
       <c r="C114" t="n">
-        <v>1000113</v>
+        <v>1000114</v>
       </c>
       <c r="D114" t="inlineStr"/>
       <c r="E114" t="inlineStr">
         <is>
-          <t>Clima</t>
+          <t>Climatici, Cambiamenti</t>
         </is>
       </c>
     </row>
@@ -2317,12 +2317,12 @@
         <v>2000001</v>
       </c>
       <c r="C115" t="n">
-        <v>1000114</v>
+        <v>1000115</v>
       </c>
       <c r="D115" t="inlineStr"/>
       <c r="E115" t="inlineStr">
         <is>
-          <t>Climatici, Cambiamenti</t>
+          <t>Climax</t>
         </is>
       </c>
     </row>
@@ -2334,12 +2334,12 @@
         <v>2000001</v>
       </c>
       <c r="C116" t="n">
-        <v>1000115</v>
+        <v>1000116</v>
       </c>
       <c r="D116" t="inlineStr"/>
       <c r="E116" t="inlineStr">
         <is>
-          <t>Climax</t>
+          <t>Club Di Roma</t>
         </is>
       </c>
     </row>
@@ -2351,12 +2351,12 @@
         <v>2000001</v>
       </c>
       <c r="C117" t="n">
-        <v>1000116</v>
+        <v>1000117</v>
       </c>
       <c r="D117" t="inlineStr"/>
       <c r="E117" t="inlineStr">
         <is>
-          <t>Club Di Roma</t>
+          <t>Cogenerazione</t>
         </is>
       </c>
     </row>
@@ -2368,12 +2368,12 @@
         <v>2000001</v>
       </c>
       <c r="C118" t="n">
-        <v>1000117</v>
+        <v>1000118</v>
       </c>
       <c r="D118" t="inlineStr"/>
       <c r="E118" t="inlineStr">
         <is>
-          <t>Cogenerazione</t>
+          <t>Collettore Solare</t>
         </is>
       </c>
     </row>
@@ -2385,12 +2385,12 @@
         <v>2000001</v>
       </c>
       <c r="C119" t="n">
-        <v>1000118</v>
+        <v>1000119</v>
       </c>
       <c r="D119" t="inlineStr"/>
       <c r="E119" t="inlineStr">
         <is>
-          <t>Collettore Solare</t>
+          <t>Combustibile derivato dai rifiuti</t>
         </is>
       </c>
     </row>
@@ -2402,12 +2402,12 @@
         <v>2000001</v>
       </c>
       <c r="C120" t="n">
-        <v>1000119</v>
+        <v>1000120</v>
       </c>
       <c r="D120" t="inlineStr"/>
       <c r="E120" t="inlineStr">
         <is>
-          <t>Combustibile derivato dai rifiuti</t>
+          <t>Combustibili Fossili</t>
         </is>
       </c>
     </row>
@@ -2419,12 +2419,12 @@
         <v>2000001</v>
       </c>
       <c r="C121" t="n">
-        <v>1000120</v>
+        <v>1000121</v>
       </c>
       <c r="D121" t="inlineStr"/>
       <c r="E121" t="inlineStr">
         <is>
-          <t>Combustibili Fossili</t>
+          <t>Comitato Di Sviluppo Locale</t>
         </is>
       </c>
     </row>
@@ -2436,12 +2436,12 @@
         <v>2000001</v>
       </c>
       <c r="C122" t="n">
-        <v>1000121</v>
+        <v>1000122</v>
       </c>
       <c r="D122" t="inlineStr"/>
       <c r="E122" t="inlineStr">
         <is>
-          <t>Comitato Di Sviluppo Locale</t>
+          <t>Command And Control</t>
         </is>
       </c>
     </row>
@@ -2453,12 +2453,12 @@
         <v>2000001</v>
       </c>
       <c r="C123" t="n">
-        <v>1000122</v>
+        <v>1000123</v>
       </c>
       <c r="D123" t="inlineStr"/>
       <c r="E123" t="inlineStr">
         <is>
-          <t>Command And Control</t>
+          <t>Compatibilità Ambientale (O Eco-Compatibilita')</t>
         </is>
       </c>
     </row>
@@ -2470,12 +2470,12 @@
         <v>2000001</v>
       </c>
       <c r="C124" t="n">
-        <v>1000123</v>
+        <v>1000124</v>
       </c>
       <c r="D124" t="inlineStr"/>
       <c r="E124" t="inlineStr">
         <is>
-          <t>Compatibilità Ambientale (O Eco-Compatibilita')</t>
+          <t>Complessità</t>
         </is>
       </c>
     </row>
@@ -2487,12 +2487,12 @@
         <v>2000001</v>
       </c>
       <c r="C125" t="n">
-        <v>1000124</v>
+        <v>1000125</v>
       </c>
       <c r="D125" t="inlineStr"/>
       <c r="E125" t="inlineStr">
         <is>
-          <t>Complessità</t>
+          <t>Componente Ambientale</t>
         </is>
       </c>
     </row>
@@ -2504,12 +2504,12 @@
         <v>2000001</v>
       </c>
       <c r="C126" t="n">
-        <v>1000125</v>
+        <v>1000126</v>
       </c>
       <c r="D126" t="inlineStr"/>
       <c r="E126" t="inlineStr">
         <is>
-          <t>Componente Ambientale</t>
+          <t>Compost</t>
         </is>
       </c>
     </row>
@@ -2521,12 +2521,12 @@
         <v>2000001</v>
       </c>
       <c r="C127" t="n">
-        <v>1000126</v>
+        <v>1000127</v>
       </c>
       <c r="D127" t="inlineStr"/>
       <c r="E127" t="inlineStr">
         <is>
-          <t>Compost</t>
+          <t>Compostaggio</t>
         </is>
       </c>
     </row>
@@ -2538,12 +2538,12 @@
         <v>2000001</v>
       </c>
       <c r="C128" t="n">
-        <v>1000127</v>
+        <v>1000128</v>
       </c>
       <c r="D128" t="inlineStr"/>
       <c r="E128" t="inlineStr">
         <is>
-          <t>Compostaggio</t>
+          <t>Comunità</t>
         </is>
       </c>
     </row>
@@ -2555,12 +2555,12 @@
         <v>2000001</v>
       </c>
       <c r="C129" t="n">
-        <v>1000128</v>
+        <v>1000129</v>
       </c>
       <c r="D129" t="inlineStr"/>
       <c r="E129" t="inlineStr">
         <is>
-          <t>Comunità</t>
+          <t>Concertazione</t>
         </is>
       </c>
     </row>
@@ -2572,12 +2572,12 @@
         <v>2000001</v>
       </c>
       <c r="C130" t="n">
-        <v>1000129</v>
+        <v>1000130</v>
       </c>
       <c r="D130" t="inlineStr"/>
       <c r="E130" t="inlineStr">
         <is>
-          <t>Concertazione</t>
+          <t>Condivisione</t>
         </is>
       </c>
     </row>
@@ -2589,12 +2589,12 @@
         <v>2000001</v>
       </c>
       <c r="C131" t="n">
-        <v>1000130</v>
+        <v>1000131</v>
       </c>
       <c r="D131" t="inlineStr"/>
       <c r="E131" t="inlineStr">
         <is>
-          <t>Condivisione</t>
+          <t>Consilience E Democrazia Cognitiva</t>
         </is>
       </c>
     </row>
@@ -2606,12 +2606,12 @@
         <v>2000001</v>
       </c>
       <c r="C132" t="n">
-        <v>1000131</v>
+        <v>1000132</v>
       </c>
       <c r="D132" t="inlineStr"/>
       <c r="E132" t="inlineStr">
         <is>
-          <t>Consilience E Democrazia Cognitiva</t>
+          <t>Green Consumerism</t>
         </is>
       </c>
     </row>
@@ -2623,12 +2623,12 @@
         <v>2000001</v>
       </c>
       <c r="C133" t="n">
-        <v>1000132</v>
+        <v>1000133</v>
       </c>
       <c r="D133" t="inlineStr"/>
       <c r="E133" t="inlineStr">
         <is>
-          <t>Green Consumerism</t>
+          <t>Contabilità Ambientale</t>
         </is>
       </c>
     </row>
@@ -2640,12 +2640,12 @@
         <v>2000001</v>
       </c>
       <c r="C134" t="n">
-        <v>1000133</v>
+        <v>1000134</v>
       </c>
       <c r="D134" t="inlineStr"/>
       <c r="E134" t="inlineStr">
         <is>
-          <t>Contabilità Ambientale</t>
+          <t>Contabilità Economica</t>
         </is>
       </c>
     </row>
@@ -2657,12 +2657,12 @@
         <v>2000001</v>
       </c>
       <c r="C135" t="n">
-        <v>1000134</v>
+        <v>1000135</v>
       </c>
       <c r="D135" t="inlineStr"/>
       <c r="E135" t="inlineStr">
         <is>
-          <t>Contabilità Economica</t>
+          <t>Conti Ambientali</t>
         </is>
       </c>
     </row>
@@ -2674,12 +2674,12 @@
         <v>2000001</v>
       </c>
       <c r="C136" t="n">
-        <v>1000135</v>
+        <v>1000136</v>
       </c>
       <c r="D136" t="inlineStr"/>
       <c r="E136" t="inlineStr">
         <is>
-          <t>Conti Ambientali</t>
+          <t>Controllo Ambientale</t>
         </is>
       </c>
     </row>
@@ -2691,12 +2691,12 @@
         <v>2000001</v>
       </c>
       <c r="C137" t="n">
-        <v>1000136</v>
+        <v>1000137</v>
       </c>
       <c r="D137" t="inlineStr"/>
       <c r="E137" t="inlineStr">
         <is>
-          <t>Controllo Ambientale</t>
+          <t>Conversione Fotovoltaica</t>
         </is>
       </c>
     </row>
@@ -2708,12 +2708,12 @@
         <v>2000001</v>
       </c>
       <c r="C138" t="n">
-        <v>1000137</v>
+        <v>1000138</v>
       </c>
       <c r="D138" t="inlineStr"/>
       <c r="E138" t="inlineStr">
         <is>
-          <t>Conversione Fotovoltaica</t>
+          <t>Cooperazione Decentrata</t>
         </is>
       </c>
     </row>
@@ -2725,12 +2725,12 @@
         <v>2000001</v>
       </c>
       <c r="C139" t="n">
-        <v>1000138</v>
+        <v>1000139</v>
       </c>
       <c r="D139" t="inlineStr"/>
       <c r="E139" t="inlineStr">
         <is>
-          <t>Cooperazione Decentrata</t>
+          <t>Cooperazione Internazionale (Allo Sviluppo)</t>
         </is>
       </c>
     </row>
@@ -2742,12 +2742,12 @@
         <v>2000001</v>
       </c>
       <c r="C140" t="n">
-        <v>1000139</v>
+        <v>1000140</v>
       </c>
       <c r="D140" t="inlineStr"/>
       <c r="E140" t="inlineStr">
         <is>
-          <t>Cooperazione Internazionale (Allo Sviluppo)</t>
+          <t>Corridoio Ecologico</t>
         </is>
       </c>
     </row>
@@ -2759,12 +2759,12 @@
         <v>2000001</v>
       </c>
       <c r="C141" t="n">
-        <v>1000140</v>
+        <v>1000141</v>
       </c>
       <c r="D141" t="inlineStr"/>
       <c r="E141" t="inlineStr">
         <is>
-          <t>Corridoio Ecologico</t>
+          <t>Costi Ambientali</t>
         </is>
       </c>
     </row>
@@ -2776,12 +2776,12 @@
         <v>2000001</v>
       </c>
       <c r="C142" t="n">
-        <v>1000141</v>
+        <v>1000142</v>
       </c>
       <c r="D142" t="inlineStr"/>
       <c r="E142" t="inlineStr">
         <is>
-          <t>Costi Ambientali</t>
+          <t>Costi Ambientali Nascosti</t>
         </is>
       </c>
     </row>
@@ -2793,12 +2793,12 @@
         <v>2000001</v>
       </c>
       <c r="C143" t="n">
-        <v>1000142</v>
+        <v>1000143</v>
       </c>
       <c r="D143" t="inlineStr"/>
       <c r="E143" t="inlineStr">
         <is>
-          <t>Costi Ambientali Nascosti</t>
+          <t>Crescita Economica Zero</t>
         </is>
       </c>
     </row>
@@ -2810,12 +2810,12 @@
         <v>2000001</v>
       </c>
       <c r="C144" t="n">
-        <v>1000143</v>
+        <v>1000144</v>
       </c>
       <c r="D144" t="inlineStr"/>
       <c r="E144" t="inlineStr">
         <is>
-          <t>Crescita Economica Zero</t>
+          <t>Cultura Ambientale</t>
         </is>
       </c>
     </row>
@@ -2827,12 +2827,12 @@
         <v>2000001</v>
       </c>
       <c r="C145" t="n">
-        <v>1000144</v>
+        <v>1000145</v>
       </c>
       <c r="D145" t="inlineStr"/>
       <c r="E145" t="inlineStr">
         <is>
-          <t>Cultura Ambientale</t>
+          <t>Cultura E Civiltà</t>
         </is>
       </c>
     </row>
@@ -2844,12 +2844,12 @@
         <v>2000001</v>
       </c>
       <c r="C146" t="n">
-        <v>1000145</v>
+        <v>1000146</v>
       </c>
       <c r="D146" t="inlineStr"/>
       <c r="E146" t="inlineStr">
         <is>
-          <t>Cultura E Civiltà</t>
+          <t>Danno Ambientale</t>
         </is>
       </c>
     </row>
@@ -2861,12 +2861,12 @@
         <v>2000001</v>
       </c>
       <c r="C147" t="n">
-        <v>1000146</v>
+        <v>1000147</v>
       </c>
       <c r="D147" t="inlineStr"/>
       <c r="E147" t="inlineStr">
         <is>
-          <t>Danno Ambientale</t>
+          <t>Decentramento</t>
         </is>
       </c>
     </row>
@@ -2878,12 +2878,12 @@
         <v>2000001</v>
       </c>
       <c r="C148" t="n">
-        <v>1000147</v>
+        <v>1000148</v>
       </c>
       <c r="D148" t="inlineStr"/>
       <c r="E148" t="inlineStr">
         <is>
-          <t>Decentramento</t>
+          <t>Decreto Ronchi</t>
         </is>
       </c>
     </row>
@@ -2895,12 +2895,12 @@
         <v>2000001</v>
       </c>
       <c r="C149" t="n">
-        <v>1000148</v>
+        <v>1000149</v>
       </c>
       <c r="D149" t="inlineStr"/>
       <c r="E149" t="inlineStr">
         <is>
-          <t>Decreto Ronchi</t>
+          <t>Deforestazione</t>
         </is>
       </c>
     </row>
@@ -2912,12 +2912,12 @@
         <v>2000001</v>
       </c>
       <c r="C150" t="n">
-        <v>1000149</v>
+        <v>1000150</v>
       </c>
       <c r="D150" t="inlineStr"/>
       <c r="E150" t="inlineStr">
         <is>
-          <t>Deforestazione</t>
+          <t>Degrado Ambientale</t>
         </is>
       </c>
     </row>
@@ -2929,12 +2929,12 @@
         <v>2000001</v>
       </c>
       <c r="C151" t="n">
-        <v>1000150</v>
+        <v>1000151</v>
       </c>
       <c r="D151" t="inlineStr"/>
       <c r="E151" t="inlineStr">
         <is>
-          <t>Degrado Ambientale</t>
+          <t>Dematerializzazione</t>
         </is>
       </c>
     </row>
@@ -2946,12 +2946,12 @@
         <v>2000001</v>
       </c>
       <c r="C152" t="n">
-        <v>1000151</v>
+        <v>1000152</v>
       </c>
       <c r="D152" t="inlineStr"/>
       <c r="E152" t="inlineStr">
         <is>
-          <t>Dematerializzazione</t>
+          <t>Desertificazione</t>
         </is>
       </c>
     </row>
@@ -2963,12 +2963,12 @@
         <v>2000001</v>
       </c>
       <c r="C153" t="n">
-        <v>1000152</v>
+        <v>1000153</v>
       </c>
       <c r="D153" t="inlineStr"/>
       <c r="E153" t="inlineStr">
         <is>
-          <t>Desertificazione</t>
+          <t>Design For Environment</t>
         </is>
       </c>
     </row>
@@ -2980,12 +2980,12 @@
         <v>2000001</v>
       </c>
       <c r="C154" t="n">
-        <v>1000153</v>
+        <v>1000154</v>
       </c>
       <c r="D154" t="inlineStr"/>
       <c r="E154" t="inlineStr">
         <is>
-          <t>Design For Environment</t>
+          <t>Dichiarazione Ambientale (Per Il Sistema Di Gestione Ambientale Emas)</t>
         </is>
       </c>
     </row>
@@ -2997,12 +2997,12 @@
         <v>2000001</v>
       </c>
       <c r="C155" t="n">
-        <v>1000154</v>
+        <v>1000155</v>
       </c>
       <c r="D155" t="inlineStr"/>
       <c r="E155" t="inlineStr">
         <is>
-          <t>Dichiarazione Ambientale (Per Il Sistema Di Gestione Ambientale Emas)</t>
+          <t>Dichiarazione Ambientale Di Prodotto</t>
         </is>
       </c>
     </row>
@@ -3014,12 +3014,12 @@
         <v>2000001</v>
       </c>
       <c r="C156" t="n">
-        <v>1000155</v>
+        <v>1000156</v>
       </c>
       <c r="D156" t="inlineStr"/>
       <c r="E156" t="inlineStr">
         <is>
-          <t>Dichiarazione Ambientale Di Prodotto</t>
+          <t>Dichiarazione Di Rio (Sull'Ambiente E Lo Sviluppo)</t>
         </is>
       </c>
     </row>
@@ -3031,12 +3031,12 @@
         <v>2000001</v>
       </c>
       <c r="C157" t="n">
-        <v>1000156</v>
+        <v>1000157</v>
       </c>
       <c r="D157" t="inlineStr"/>
       <c r="E157" t="inlineStr">
         <is>
-          <t>Dichiarazione Di Rio (Sull'Ambiente E Lo Sviluppo)</t>
+          <t>Dipendenza Energetica</t>
         </is>
       </c>
     </row>
@@ -3048,12 +3048,12 @@
         <v>2000001</v>
       </c>
       <c r="C158" t="n">
-        <v>1000157</v>
+        <v>1000158</v>
       </c>
       <c r="D158" t="inlineStr"/>
       <c r="E158" t="inlineStr">
         <is>
-          <t>Dipendenza Energetica</t>
+          <t>Direttiva Habitat</t>
         </is>
       </c>
     </row>
@@ -3065,12 +3065,12 @@
         <v>2000001</v>
       </c>
       <c r="C159" t="n">
-        <v>1000158</v>
+        <v>1000159</v>
       </c>
       <c r="D159" t="inlineStr"/>
       <c r="E159" t="inlineStr">
         <is>
-          <t>Direttiva Habitat</t>
+          <t>Direttive Ue</t>
         </is>
       </c>
     </row>
@@ -3082,12 +3082,12 @@
         <v>2000001</v>
       </c>
       <c r="C160" t="n">
-        <v>1000159</v>
+        <v>1000160</v>
       </c>
       <c r="D160" t="inlineStr"/>
       <c r="E160" t="inlineStr">
         <is>
-          <t>Direttive Ue</t>
+          <t>Dismissione</t>
         </is>
       </c>
     </row>
@@ -3099,12 +3099,12 @@
         <v>2000001</v>
       </c>
       <c r="C161" t="n">
-        <v>1000160</v>
+        <v>1000161</v>
       </c>
       <c r="D161" t="inlineStr"/>
       <c r="E161" t="inlineStr">
         <is>
-          <t>Dismissione</t>
+          <t>Dissesti Idrogeologici</t>
         </is>
       </c>
     </row>
@@ -3116,12 +3116,12 @@
         <v>2000001</v>
       </c>
       <c r="C162" t="n">
-        <v>1000161</v>
+        <v>1000162</v>
       </c>
       <c r="D162" t="inlineStr"/>
       <c r="E162" t="inlineStr">
         <is>
-          <t>Dissesti Idrogeologici</t>
+          <t>Ecoaudit</t>
         </is>
       </c>
     </row>
@@ -3133,12 +3133,12 @@
         <v>2000001</v>
       </c>
       <c r="C163" t="n">
-        <v>1000162</v>
+        <v>1000163</v>
       </c>
       <c r="D163" t="inlineStr"/>
       <c r="E163" t="inlineStr">
         <is>
-          <t>Ecoaudit</t>
+          <t>Ecodesign</t>
         </is>
       </c>
     </row>
@@ -3150,12 +3150,12 @@
         <v>2000001</v>
       </c>
       <c r="C164" t="n">
-        <v>1000163</v>
+        <v>1000164</v>
       </c>
       <c r="D164" t="inlineStr"/>
       <c r="E164" t="inlineStr">
         <is>
-          <t>Ecodesign</t>
+          <t>Ecodumping</t>
         </is>
       </c>
     </row>
@@ -3167,12 +3167,12 @@
         <v>2000001</v>
       </c>
       <c r="C165" t="n">
-        <v>1000164</v>
+        <v>1000165</v>
       </c>
       <c r="D165" t="inlineStr"/>
       <c r="E165" t="inlineStr">
         <is>
-          <t>Ecodumping</t>
+          <t>Ecogestione</t>
         </is>
       </c>
     </row>
@@ -3184,12 +3184,12 @@
         <v>2000001</v>
       </c>
       <c r="C166" t="n">
-        <v>1000165</v>
+        <v>1000166</v>
       </c>
       <c r="D166" t="inlineStr"/>
       <c r="E166" t="inlineStr">
         <is>
-          <t>Ecogestione</t>
+          <t>Eco-Innovatori</t>
         </is>
       </c>
     </row>
@@ -3201,12 +3201,12 @@
         <v>2000001</v>
       </c>
       <c r="C167" t="n">
-        <v>1000166</v>
+        <v>1000167</v>
       </c>
       <c r="D167" t="inlineStr"/>
       <c r="E167" t="inlineStr">
         <is>
-          <t>Eco-Innovatori</t>
+          <t>Eco-Labelling</t>
         </is>
       </c>
     </row>
@@ -3218,12 +3218,12 @@
         <v>2000001</v>
       </c>
       <c r="C168" t="n">
-        <v>1000167</v>
+        <v>1000168</v>
       </c>
       <c r="D168" t="inlineStr"/>
       <c r="E168" t="inlineStr">
         <is>
-          <t>Eco-Labelling</t>
+          <t>Eco-Leader</t>
         </is>
       </c>
     </row>
@@ -3235,12 +3235,12 @@
         <v>2000001</v>
       </c>
       <c r="C169" t="n">
-        <v>1000168</v>
+        <v>1000169</v>
       </c>
       <c r="D169" t="inlineStr"/>
       <c r="E169" t="inlineStr">
         <is>
-          <t>Eco-Leader</t>
+          <t>Ecologia</t>
         </is>
       </c>
     </row>
@@ -3252,12 +3252,12 @@
         <v>2000001</v>
       </c>
       <c r="C170" t="n">
-        <v>1000169</v>
+        <v>1000170</v>
       </c>
       <c r="D170" t="inlineStr"/>
       <c r="E170" t="inlineStr">
         <is>
-          <t>Ecologia</t>
+          <t>Ecologia Domestica</t>
         </is>
       </c>
     </row>
@@ -3269,12 +3269,12 @@
         <v>2000001</v>
       </c>
       <c r="C171" t="n">
-        <v>1000170</v>
+        <v>1000171</v>
       </c>
       <c r="D171" t="inlineStr"/>
       <c r="E171" t="inlineStr">
         <is>
-          <t>Ecologia Domestica</t>
+          <t>Ecologia Industriale</t>
         </is>
       </c>
     </row>
@@ -3286,12 +3286,12 @@
         <v>2000001</v>
       </c>
       <c r="C172" t="n">
-        <v>1000171</v>
+        <v>1000172</v>
       </c>
       <c r="D172" t="inlineStr"/>
       <c r="E172" t="inlineStr">
         <is>
-          <t>Ecologia Industriale</t>
+          <t>Economia Sostenibile</t>
         </is>
       </c>
     </row>
@@ -3303,12 +3303,12 @@
         <v>2000001</v>
       </c>
       <c r="C173" t="n">
-        <v>1000172</v>
+        <v>1000173</v>
       </c>
       <c r="D173" t="inlineStr"/>
       <c r="E173" t="inlineStr">
         <is>
-          <t>Economia Sostenibile</t>
+          <t>Ecosistema Antropico</t>
         </is>
       </c>
     </row>
@@ -3320,12 +3320,12 @@
         <v>2000001</v>
       </c>
       <c r="C174" t="n">
-        <v>1000173</v>
+        <v>1000174</v>
       </c>
       <c r="D174" t="inlineStr"/>
       <c r="E174" t="inlineStr">
         <is>
-          <t>Ecosistema Antropico</t>
+          <t>Ecosistema Naturale</t>
         </is>
       </c>
     </row>
@@ -3337,12 +3337,12 @@
         <v>2000001</v>
       </c>
       <c r="C175" t="n">
-        <v>1000174</v>
+        <v>1000175</v>
       </c>
       <c r="D175" t="inlineStr"/>
       <c r="E175" t="inlineStr">
         <is>
-          <t>Ecosistema Naturale</t>
+          <t>Ecosistema O Sistema Ecologico</t>
         </is>
       </c>
     </row>
@@ -3354,12 +3354,12 @@
         <v>2000001</v>
       </c>
       <c r="C176" t="n">
-        <v>1000175</v>
+        <v>1000176</v>
       </c>
       <c r="D176" t="inlineStr"/>
       <c r="E176" t="inlineStr">
         <is>
-          <t>Ecosistema O Sistema Ecologico</t>
+          <t>Ecosviluppo</t>
         </is>
       </c>
     </row>
@@ -3371,12 +3371,12 @@
         <v>2000001</v>
       </c>
       <c r="C177" t="n">
-        <v>1000176</v>
+        <v>1000177</v>
       </c>
       <c r="D177" t="inlineStr"/>
       <c r="E177" t="inlineStr">
         <is>
-          <t>Ecosviluppo</t>
+          <t>Ecovillaggi</t>
         </is>
       </c>
     </row>
@@ -3388,12 +3388,12 @@
         <v>2000001</v>
       </c>
       <c r="C178" t="n">
-        <v>1000177</v>
+        <v>1000178</v>
       </c>
       <c r="D178" t="inlineStr"/>
       <c r="E178" t="inlineStr">
         <is>
-          <t>Ecovillaggi</t>
+          <t>Educazione Ambientale</t>
         </is>
       </c>
     </row>
@@ -3405,12 +3405,12 @@
         <v>2000001</v>
       </c>
       <c r="C179" t="n">
-        <v>1000178</v>
+        <v>1000179</v>
       </c>
       <c r="D179" t="inlineStr"/>
       <c r="E179" t="inlineStr">
         <is>
-          <t>Educazione Ambientale</t>
+          <t>Effetti A Breve O A Lungo Termine</t>
         </is>
       </c>
     </row>
@@ -3422,12 +3422,12 @@
         <v>2000001</v>
       </c>
       <c r="C180" t="n">
-        <v>1000179</v>
+        <v>1000180</v>
       </c>
       <c r="D180" t="inlineStr"/>
       <c r="E180" t="inlineStr">
         <is>
-          <t>Effetti A Breve O A Lungo Termine</t>
+          <t>Effetti Ambientali</t>
         </is>
       </c>
     </row>
@@ -3439,12 +3439,12 @@
         <v>2000001</v>
       </c>
       <c r="C181" t="n">
-        <v>1000180</v>
+        <v>1000181</v>
       </c>
       <c r="D181" t="inlineStr"/>
       <c r="E181" t="inlineStr">
         <is>
-          <t>Effetti Ambientali</t>
+          <t>Effetti Ambientali Globali</t>
         </is>
       </c>
     </row>
@@ -3456,12 +3456,12 @@
         <v>2000001</v>
       </c>
       <c r="C182" t="n">
-        <v>1000181</v>
+        <v>1000182</v>
       </c>
       <c r="D182" t="inlineStr"/>
       <c r="E182" t="inlineStr">
         <is>
-          <t>Effetti Ambientali Globali</t>
+          <t>Effetto Fotovoltaico</t>
         </is>
       </c>
     </row>
@@ -3473,12 +3473,12 @@
         <v>2000001</v>
       </c>
       <c r="C183" t="n">
-        <v>1000182</v>
+        <v>1000183</v>
       </c>
       <c r="D183" t="inlineStr"/>
       <c r="E183" t="inlineStr">
         <is>
-          <t>Effetto Fotovoltaico</t>
+          <t>Effetto Serra</t>
         </is>
       </c>
     </row>
@@ -3490,12 +3490,12 @@
         <v>2000001</v>
       </c>
       <c r="C184" t="n">
-        <v>1000183</v>
+        <v>1000184</v>
       </c>
       <c r="D184" t="inlineStr"/>
       <c r="E184" t="inlineStr">
         <is>
-          <t>Effetto Serra</t>
+          <t>Efficienza Ambientale</t>
         </is>
       </c>
     </row>
@@ -3507,12 +3507,12 @@
         <v>2000001</v>
       </c>
       <c r="C185" t="n">
-        <v>1000184</v>
+        <v>1000185</v>
       </c>
       <c r="D185" t="inlineStr"/>
       <c r="E185" t="inlineStr">
         <is>
-          <t>Efficienza Ambientale</t>
+          <t>Efficienza Energetica</t>
         </is>
       </c>
     </row>
@@ -3524,12 +3524,12 @@
         <v>2000001</v>
       </c>
       <c r="C186" t="n">
-        <v>1000185</v>
+        <v>1000186</v>
       </c>
       <c r="D186" t="inlineStr"/>
       <c r="E186" t="inlineStr">
         <is>
-          <t>Efficienza Energetica</t>
+          <t>Emergia O Embodied Energy</t>
         </is>
       </c>
     </row>
@@ -3541,12 +3541,12 @@
         <v>2000001</v>
       </c>
       <c r="C187" t="n">
-        <v>1000186</v>
+        <v>1000187</v>
       </c>
       <c r="D187" t="inlineStr"/>
       <c r="E187" t="inlineStr">
         <is>
-          <t>Emergia O Embodied Energy</t>
+          <t>Emergence</t>
         </is>
       </c>
     </row>
@@ -3558,12 +3558,12 @@
         <v>2000001</v>
       </c>
       <c r="C188" t="n">
-        <v>1000187</v>
+        <v>1000188</v>
       </c>
       <c r="D188" t="inlineStr"/>
       <c r="E188" t="inlineStr">
         <is>
-          <t>Emergence</t>
+          <t>Emission Trading</t>
         </is>
       </c>
     </row>
@@ -3575,12 +3575,12 @@
         <v>2000001</v>
       </c>
       <c r="C189" t="n">
-        <v>1000188</v>
+        <v>1000189</v>
       </c>
       <c r="D189" t="inlineStr"/>
       <c r="E189" t="inlineStr">
         <is>
-          <t>Emission Trading</t>
+          <t>Emissione</t>
         </is>
       </c>
     </row>
@@ -3592,12 +3592,12 @@
         <v>2000001</v>
       </c>
       <c r="C190" t="n">
-        <v>1000189</v>
+        <v>1000190</v>
       </c>
       <c r="D190" t="inlineStr"/>
       <c r="E190" t="inlineStr">
         <is>
-          <t>Emissione</t>
+          <t>Empowerment</t>
         </is>
       </c>
     </row>
@@ -3609,12 +3609,12 @@
         <v>2000001</v>
       </c>
       <c r="C191" t="n">
-        <v>1000190</v>
+        <v>1000191</v>
       </c>
       <c r="D191" t="inlineStr"/>
       <c r="E191" t="inlineStr">
         <is>
-          <t>Empowerment</t>
+          <t>Energia</t>
         </is>
       </c>
     </row>
@@ -3626,12 +3626,12 @@
         <v>2000001</v>
       </c>
       <c r="C192" t="n">
-        <v>1000191</v>
+        <v>1000192</v>
       </c>
       <c r="D192" t="inlineStr"/>
       <c r="E192" t="inlineStr">
         <is>
-          <t>Energia</t>
+          <t>Energia Geotermica</t>
         </is>
       </c>
     </row>
@@ -3643,12 +3643,12 @@
         <v>2000001</v>
       </c>
       <c r="C193" t="n">
-        <v>1000191</v>
+        <v>1000193</v>
       </c>
       <c r="D193" t="inlineStr"/>
       <c r="E193" t="inlineStr">
         <is>
-          <t>Energia</t>
+          <t>Energia Alternativa</t>
         </is>
       </c>
     </row>
@@ -3660,12 +3660,12 @@
         <v>2000001</v>
       </c>
       <c r="C194" t="n">
-        <v>1000193</v>
+        <v>1000194</v>
       </c>
       <c r="D194" t="inlineStr"/>
       <c r="E194" t="inlineStr">
         <is>
-          <t>Energia Alternativa</t>
+          <t>Energia Eolica</t>
         </is>
       </c>
     </row>
@@ -3677,12 +3677,12 @@
         <v>2000001</v>
       </c>
       <c r="C195" t="n">
-        <v>1000194</v>
+        <v>1000195</v>
       </c>
       <c r="D195" t="inlineStr"/>
       <c r="E195" t="inlineStr">
         <is>
-          <t>Energia Eolica</t>
+          <t>Energia Idraulica</t>
         </is>
       </c>
     </row>
@@ -3694,12 +3694,12 @@
         <v>2000001</v>
       </c>
       <c r="C196" t="n">
-        <v>1000192</v>
+        <v>1000196</v>
       </c>
       <c r="D196" t="inlineStr"/>
       <c r="E196" t="inlineStr">
         <is>
-          <t>Energia Geotermica</t>
+          <t>Energia Solare</t>
         </is>
       </c>
     </row>
@@ -3711,12 +3711,12 @@
         <v>2000001</v>
       </c>
       <c r="C197" t="n">
-        <v>1000195</v>
+        <v>1000197</v>
       </c>
       <c r="D197" t="inlineStr"/>
       <c r="E197" t="inlineStr">
         <is>
-          <t>Energia Idraulica</t>
+          <t>Energia Nucleare</t>
         </is>
       </c>
     </row>
@@ -3728,12 +3728,12 @@
         <v>2000001</v>
       </c>
       <c r="C198" t="n">
-        <v>1000197</v>
+        <v>1000198</v>
       </c>
       <c r="D198" t="inlineStr"/>
       <c r="E198" t="inlineStr">
         <is>
-          <t>Energia Nucleare</t>
+          <t>Energia Rinnovabile</t>
         </is>
       </c>
     </row>
@@ -3745,12 +3745,12 @@
         <v>2000001</v>
       </c>
       <c r="C199" t="n">
-        <v>1000198</v>
+        <v>1000199</v>
       </c>
       <c r="D199" t="inlineStr"/>
       <c r="E199" t="inlineStr">
         <is>
-          <t>Energia Rinnovabile</t>
+          <t>Energie Alternative</t>
         </is>
       </c>
     </row>
@@ -3762,12 +3762,12 @@
         <v>2000001</v>
       </c>
       <c r="C200" t="n">
-        <v>1000196</v>
+        <v>1000201</v>
       </c>
       <c r="D200" t="inlineStr"/>
       <c r="E200" t="inlineStr">
         <is>
-          <t>Energia Solare</t>
+          <t>Energy Audit</t>
         </is>
       </c>
     </row>
@@ -3779,12 +3779,12 @@
         <v>2000001</v>
       </c>
       <c r="C201" t="n">
-        <v>1000199</v>
+        <v>1000202</v>
       </c>
       <c r="D201" t="inlineStr"/>
       <c r="E201" t="inlineStr">
         <is>
-          <t>Energie Alternative</t>
+          <t>Entropia</t>
         </is>
       </c>
     </row>
@@ -3796,12 +3796,12 @@
         <v>2000001</v>
       </c>
       <c r="C202" t="n">
-        <v>1000201</v>
+        <v>1000203</v>
       </c>
       <c r="D202" t="inlineStr"/>
       <c r="E202" t="inlineStr">
         <is>
-          <t>Energy Audit</t>
+          <t>Environmental Condition Indicators</t>
         </is>
       </c>
     </row>
@@ -3813,12 +3813,12 @@
         <v>2000001</v>
       </c>
       <c r="C203" t="n">
-        <v>1000202</v>
+        <v>1000204</v>
       </c>
       <c r="D203" t="inlineStr"/>
       <c r="E203" t="inlineStr">
         <is>
-          <t>Entropia</t>
+          <t>Environmental Performance Indicators</t>
         </is>
       </c>
     </row>
@@ -3830,12 +3830,12 @@
         <v>2000001</v>
       </c>
       <c r="C204" t="n">
-        <v>1000203</v>
+        <v>1000205</v>
       </c>
       <c r="D204" t="inlineStr"/>
       <c r="E204" t="inlineStr">
         <is>
-          <t>Environmental Condition Indicators</t>
+          <t>Equilibrio</t>
         </is>
       </c>
     </row>
@@ -3847,12 +3847,12 @@
         <v>2000001</v>
       </c>
       <c r="C205" t="n">
-        <v>1000204</v>
+        <v>1000206</v>
       </c>
       <c r="D205" t="inlineStr"/>
       <c r="E205" t="inlineStr">
         <is>
-          <t>Environmental Performance Indicators</t>
+          <t>Equità</t>
         </is>
       </c>
     </row>
@@ -3864,12 +3864,12 @@
         <v>2000001</v>
       </c>
       <c r="C206" t="n">
-        <v>1000205</v>
+        <v>1000207</v>
       </c>
       <c r="D206" t="inlineStr"/>
       <c r="E206" t="inlineStr">
         <is>
-          <t>Equilibrio</t>
+          <t>Equità Intergenerazionale</t>
         </is>
       </c>
     </row>
@@ -3881,12 +3881,12 @@
         <v>2000001</v>
       </c>
       <c r="C207" t="n">
-        <v>1000206</v>
+        <v>1000208</v>
       </c>
       <c r="D207" t="inlineStr"/>
       <c r="E207" t="inlineStr">
         <is>
-          <t>Equità</t>
+          <t>Ergonomia</t>
         </is>
       </c>
     </row>
@@ -3898,12 +3898,12 @@
         <v>2000001</v>
       </c>
       <c r="C208" t="n">
-        <v>1000207</v>
+        <v>1000209</v>
       </c>
       <c r="D208" t="inlineStr"/>
       <c r="E208" t="inlineStr">
         <is>
-          <t>Equità Intergenerazionale</t>
+          <t>Esternalità</t>
         </is>
       </c>
     </row>
@@ -3915,12 +3915,12 @@
         <v>2000001</v>
       </c>
       <c r="C209" t="n">
-        <v>1000208</v>
+        <v>1000210</v>
       </c>
       <c r="D209" t="inlineStr"/>
       <c r="E209" t="inlineStr">
         <is>
-          <t>Ergonomia</t>
+          <t>Esternalità Ambientali</t>
         </is>
       </c>
     </row>
@@ -3932,12 +3932,12 @@
         <v>2000001</v>
       </c>
       <c r="C210" t="n">
-        <v>1000209</v>
+        <v>1000211</v>
       </c>
       <c r="D210" t="inlineStr"/>
       <c r="E210" t="inlineStr">
         <is>
-          <t>Esternalità</t>
+          <t>Etica</t>
         </is>
       </c>
     </row>
@@ -3949,12 +3949,12 @@
         <v>2000001</v>
       </c>
       <c r="C211" t="n">
-        <v>1000210</v>
+        <v>1000212</v>
       </c>
       <c r="D211" t="inlineStr"/>
       <c r="E211" t="inlineStr">
         <is>
-          <t>Esternalità Ambientali</t>
+          <t>European Awareness Scenario Workshop</t>
         </is>
       </c>
     </row>
@@ -3966,12 +3966,12 @@
         <v>2000001</v>
       </c>
       <c r="C212" t="n">
-        <v>1000211</v>
+        <v>1000213</v>
       </c>
       <c r="D212" t="inlineStr"/>
       <c r="E212" t="inlineStr">
         <is>
-          <t>Etica</t>
+          <t>European Common Indicators</t>
         </is>
       </c>
     </row>
@@ -3983,12 +3983,12 @@
         <v>2000001</v>
       </c>
       <c r="C213" t="n">
-        <v>1000212</v>
+        <v>1000214</v>
       </c>
       <c r="D213" t="inlineStr"/>
       <c r="E213" t="inlineStr">
         <is>
-          <t>European Awareness Scenario Workshop</t>
+          <t>Eutrofizzazione</t>
         </is>
       </c>
     </row>
@@ -4000,12 +4000,12 @@
         <v>2000001</v>
       </c>
       <c r="C214" t="n">
-        <v>1000213</v>
+        <v>1000215</v>
       </c>
       <c r="D214" t="inlineStr"/>
       <c r="E214" t="inlineStr">
         <is>
-          <t>European Common Indicators</t>
+          <t>Evoluzione Degli Ecosistemi</t>
         </is>
       </c>
     </row>
@@ -4017,12 +4017,12 @@
         <v>2000001</v>
       </c>
       <c r="C215" t="n">
-        <v>1000214</v>
+        <v>1000216</v>
       </c>
       <c r="D215" t="inlineStr"/>
       <c r="E215" t="inlineStr">
         <is>
-          <t>Eutrofizzazione</t>
+          <t>Ex Situ</t>
         </is>
       </c>
     </row>
@@ -4034,12 +4034,12 @@
         <v>2000001</v>
       </c>
       <c r="C216" t="n">
-        <v>1000215</v>
+        <v>1000217</v>
       </c>
       <c r="D216" t="inlineStr"/>
       <c r="E216" t="inlineStr">
         <is>
-          <t>Evoluzione Degli Ecosistemi</t>
+          <t>Facilitatore</t>
         </is>
       </c>
     </row>
@@ -4051,12 +4051,12 @@
         <v>2000001</v>
       </c>
       <c r="C217" t="n">
-        <v>1000216</v>
+        <v>1000218</v>
       </c>
       <c r="D217" t="inlineStr"/>
       <c r="E217" t="inlineStr">
         <is>
-          <t>Ex Situ</t>
+          <t>Fattore D'Impatto Ambientale</t>
         </is>
       </c>
     </row>
@@ -4068,12 +4068,12 @@
         <v>2000001</v>
       </c>
       <c r="C218" t="n">
-        <v>1000217</v>
+        <v>1000219</v>
       </c>
       <c r="D218" t="inlineStr"/>
       <c r="E218" t="inlineStr">
         <is>
-          <t>Facilitatore</t>
+          <t>Fattori Biotici</t>
         </is>
       </c>
     </row>
@@ -4085,12 +4085,12 @@
         <v>2000001</v>
       </c>
       <c r="C219" t="n">
-        <v>1000218</v>
+        <v>1000220</v>
       </c>
       <c r="D219" t="inlineStr"/>
       <c r="E219" t="inlineStr">
         <is>
-          <t>Fattore D'Impatto Ambientale</t>
+          <t>Fattori Di Pressione</t>
         </is>
       </c>
     </row>
@@ -4102,12 +4102,12 @@
         <v>2000001</v>
       </c>
       <c r="C220" t="n">
-        <v>1000219</v>
+        <v>1000221</v>
       </c>
       <c r="D220" t="inlineStr"/>
       <c r="E220" t="inlineStr">
         <is>
-          <t>Fattori Biotici</t>
+          <t>Fauna</t>
         </is>
       </c>
     </row>
@@ -4119,12 +4119,12 @@
         <v>2000001</v>
       </c>
       <c r="C221" t="n">
-        <v>1000220</v>
+        <v>1000222</v>
       </c>
       <c r="D221" t="inlineStr"/>
       <c r="E221" t="inlineStr">
         <is>
-          <t>Fattori Di Pressione</t>
+          <t>Feedback</t>
         </is>
       </c>
     </row>
@@ -4136,12 +4136,12 @@
         <v>2000001</v>
       </c>
       <c r="C222" t="n">
-        <v>1000221</v>
+        <v>1000223</v>
       </c>
       <c r="D222" t="inlineStr"/>
       <c r="E222" t="inlineStr">
         <is>
-          <t>Fauna</t>
+          <t>Feng Shui</t>
         </is>
       </c>
     </row>
@@ -4153,12 +4153,12 @@
         <v>2000001</v>
       </c>
       <c r="C223" t="n">
-        <v>1000222</v>
+        <v>1000224</v>
       </c>
       <c r="D223" t="inlineStr"/>
       <c r="E223" t="inlineStr">
         <is>
-          <t>Feedback</t>
+          <t>Filosofia Ambientale</t>
         </is>
       </c>
     </row>
@@ -4170,12 +4170,12 @@
         <v>2000001</v>
       </c>
       <c r="C224" t="n">
-        <v>1000223</v>
+        <v>1000225</v>
       </c>
       <c r="D224" t="inlineStr"/>
       <c r="E224" t="inlineStr">
         <is>
-          <t>Feng Shui</t>
+          <t>Finanza Etica</t>
         </is>
       </c>
     </row>
@@ -4187,12 +4187,12 @@
         <v>2000001</v>
       </c>
       <c r="C225" t="n">
-        <v>1000224</v>
+        <v>1000226</v>
       </c>
       <c r="D225" t="inlineStr"/>
       <c r="E225" t="inlineStr">
         <is>
-          <t>Filosofia Ambientale</t>
+          <t>Fiscalità Ambientale</t>
         </is>
       </c>
     </row>
@@ -4204,12 +4204,12 @@
         <v>2000001</v>
       </c>
       <c r="C226" t="n">
-        <v>1000225</v>
+        <v>1000227</v>
       </c>
       <c r="D226" t="inlineStr"/>
       <c r="E226" t="inlineStr">
         <is>
-          <t>Finanza Etica</t>
+          <t>Fitodepurazione</t>
         </is>
       </c>
     </row>
@@ -4221,12 +4221,12 @@
         <v>2000001</v>
       </c>
       <c r="C227" t="n">
-        <v>1000226</v>
+        <v>1000228</v>
       </c>
       <c r="D227" t="inlineStr"/>
       <c r="E227" t="inlineStr">
         <is>
-          <t>Fiscalità Ambientale</t>
+          <t>Fitorisanamento</t>
         </is>
       </c>
     </row>
@@ -4238,12 +4238,12 @@
         <v>2000001</v>
       </c>
       <c r="C228" t="n">
-        <v>1000227</v>
+        <v>1000229</v>
       </c>
       <c r="D228" t="inlineStr"/>
       <c r="E228" t="inlineStr">
         <is>
-          <t>Fitodepurazione</t>
+          <t>Fondi Ecologici</t>
         </is>
       </c>
     </row>
@@ -4255,12 +4255,12 @@
         <v>2000001</v>
       </c>
       <c r="C229" t="n">
-        <v>1000228</v>
+        <v>1000230</v>
       </c>
       <c r="D229" t="inlineStr"/>
       <c r="E229" t="inlineStr">
         <is>
-          <t>Fitorisanamento</t>
+          <t>Fondi Strutturali E Fondo Di Coesione</t>
         </is>
       </c>
     </row>
@@ -4272,12 +4272,12 @@
         <v>2000001</v>
       </c>
       <c r="C230" t="n">
-        <v>1000229</v>
+        <v>1000231</v>
       </c>
       <c r="D230" t="inlineStr"/>
       <c r="E230" t="inlineStr">
         <is>
-          <t>Fondi Ecologici</t>
+          <t>Fondo Europeo Agricolo Di Orientamento E Garanzia</t>
         </is>
       </c>
     </row>
@@ -4289,12 +4289,12 @@
         <v>2000001</v>
       </c>
       <c r="C231" t="n">
-        <v>1000230</v>
+        <v>1000232</v>
       </c>
       <c r="D231" t="inlineStr"/>
       <c r="E231" t="inlineStr">
         <is>
-          <t>Fondi Strutturali E Fondo Di Coesione</t>
+          <t>Fondo Europeo Di Sviluppo Regionale</t>
         </is>
       </c>
     </row>
@@ -4306,12 +4306,12 @@
         <v>2000001</v>
       </c>
       <c r="C232" t="n">
-        <v>1000231</v>
+        <v>1000233</v>
       </c>
       <c r="D232" t="inlineStr"/>
       <c r="E232" t="inlineStr">
         <is>
-          <t>Fondo Europeo Agricolo Di Orientamento E Garanzia</t>
+          <t>Fondo Europeo Per Gli Investimenti</t>
         </is>
       </c>
     </row>
@@ -4323,12 +4323,12 @@
         <v>2000001</v>
       </c>
       <c r="C233" t="n">
-        <v>1000232</v>
+        <v>1000234</v>
       </c>
       <c r="D233" t="inlineStr"/>
       <c r="E233" t="inlineStr">
         <is>
-          <t>Fondo Europeo Di Sviluppo Regionale</t>
+          <t>Fonti Assimilate</t>
         </is>
       </c>
     </row>
@@ -4340,12 +4340,12 @@
         <v>2000001</v>
       </c>
       <c r="C234" t="n">
-        <v>1000233</v>
+        <v>1000235</v>
       </c>
       <c r="D234" t="inlineStr"/>
       <c r="E234" t="inlineStr">
         <is>
-          <t>Fondo Europeo Per Gli Investimenti</t>
+          <t>Fonti Rinnovabili</t>
         </is>
       </c>
     </row>
@@ -4357,12 +4357,12 @@
         <v>2000001</v>
       </c>
       <c r="C235" t="n">
-        <v>1000234</v>
+        <v>1000237</v>
       </c>
       <c r="D235" t="inlineStr"/>
       <c r="E235" t="inlineStr">
         <is>
-          <t>Fonti Assimilate</t>
+          <t>Formazione Di Rete</t>
         </is>
       </c>
     </row>
@@ -4374,12 +4374,12 @@
         <v>2000001</v>
       </c>
       <c r="C236" t="n">
-        <v>1000235</v>
+        <v>1000238</v>
       </c>
       <c r="D236" t="inlineStr"/>
       <c r="E236" t="inlineStr">
         <is>
-          <t>Fonti Rinnovabili</t>
+          <t>Gas Serra</t>
         </is>
       </c>
     </row>
@@ -4391,12 +4391,12 @@
         <v>2000001</v>
       </c>
       <c r="C237" t="n">
-        <v>1000085</v>
+        <v>1000239</v>
       </c>
       <c r="D237" t="inlineStr"/>
       <c r="E237" t="inlineStr">
         <is>
-          <t>Capacity Building</t>
+          <t>Geobiologia</t>
         </is>
       </c>
     </row>
@@ -4408,12 +4408,12 @@
         <v>2000001</v>
       </c>
       <c r="C238" t="n">
-        <v>1000237</v>
+        <v>1000240</v>
       </c>
       <c r="D238" t="inlineStr"/>
       <c r="E238" t="inlineStr">
         <is>
-          <t>Formazione Di Rete</t>
+          <t>Gestione Del Bene Durante L'Intero Ciclo Di Vita</t>
         </is>
       </c>
     </row>
@@ -4425,12 +4425,12 @@
         <v>2000001</v>
       </c>
       <c r="C239" t="n">
-        <v>1000238</v>
+        <v>1000241</v>
       </c>
       <c r="D239" t="inlineStr"/>
       <c r="E239" t="inlineStr">
         <is>
-          <t>Gas Serra</t>
+          <t>Demand Management</t>
         </is>
       </c>
     </row>
@@ -4442,12 +4442,12 @@
         <v>2000001</v>
       </c>
       <c r="C240" t="n">
-        <v>1000239</v>
+        <v>1000242</v>
       </c>
       <c r="D240" t="inlineStr"/>
       <c r="E240" t="inlineStr">
         <is>
-          <t>Geobiologia</t>
+          <t>Gestione Integrata</t>
         </is>
       </c>
     </row>
@@ -4459,12 +4459,12 @@
         <v>2000001</v>
       </c>
       <c r="C241" t="n">
-        <v>1000240</v>
+        <v>1000243</v>
       </c>
       <c r="D241" t="inlineStr"/>
       <c r="E241" t="inlineStr">
         <is>
-          <t>Gestione Del Bene Durante L'Intero Ciclo Di Vita</t>
+          <t>Global Reporting Iniziative</t>
         </is>
       </c>
     </row>
@@ -4476,12 +4476,12 @@
         <v>2000001</v>
       </c>
       <c r="C242" t="n">
-        <v>1000241</v>
+        <v>1000244</v>
       </c>
       <c r="D242" t="inlineStr"/>
       <c r="E242" t="inlineStr">
         <is>
-          <t>Demand Management</t>
+          <t>Globalizzazione</t>
         </is>
       </c>
     </row>
@@ -4493,12 +4493,12 @@
         <v>2000001</v>
       </c>
       <c r="C243" t="n">
-        <v>1000242</v>
+        <v>1000245</v>
       </c>
       <c r="D243" t="inlineStr"/>
       <c r="E243" t="inlineStr">
         <is>
-          <t>Gestione Integrata</t>
+          <t>Globalizzazione Dell'Economia</t>
         </is>
       </c>
     </row>
@@ -4510,12 +4510,12 @@
         <v>2000001</v>
       </c>
       <c r="C244" t="n">
-        <v>1000243</v>
+        <v>1000246</v>
       </c>
       <c r="D244" t="inlineStr"/>
       <c r="E244" t="inlineStr">
         <is>
-          <t>Global Reporting Iniziative</t>
+          <t>Glocacità</t>
         </is>
       </c>
     </row>
@@ -4527,12 +4527,12 @@
         <v>2000001</v>
       </c>
       <c r="C245" t="n">
-        <v>1000244</v>
+        <v>1000247</v>
       </c>
       <c r="D245" t="inlineStr"/>
       <c r="E245" t="inlineStr">
         <is>
-          <t>Globalizzazione</t>
+          <t>Governance</t>
         </is>
       </c>
     </row>
@@ -4544,12 +4544,12 @@
         <v>2000001</v>
       </c>
       <c r="C246" t="n">
-        <v>1000245</v>
+        <v>1000248</v>
       </c>
       <c r="D246" t="inlineStr"/>
       <c r="E246" t="inlineStr">
         <is>
-          <t>Globalizzazione Dell'Economia</t>
+          <t>Green Public Procurement</t>
         </is>
       </c>
     </row>
@@ -4561,61 +4561,10 @@
         <v>2000001</v>
       </c>
       <c r="C247" t="n">
-        <v>1000246</v>
+        <v>1000249</v>
       </c>
       <c r="D247" t="inlineStr"/>
       <c r="E247" t="inlineStr">
-        <is>
-          <t>Glocacità</t>
-        </is>
-      </c>
-    </row>
-    <row r="248">
-      <c r="A248" s="1" t="n">
-        <v>246</v>
-      </c>
-      <c r="B248" t="n">
-        <v>2000001</v>
-      </c>
-      <c r="C248" t="n">
-        <v>1000247</v>
-      </c>
-      <c r="D248" t="inlineStr"/>
-      <c r="E248" t="inlineStr">
-        <is>
-          <t>Governance</t>
-        </is>
-      </c>
-    </row>
-    <row r="249">
-      <c r="A249" s="1" t="n">
-        <v>247</v>
-      </c>
-      <c r="B249" t="n">
-        <v>2000001</v>
-      </c>
-      <c r="C249" t="n">
-        <v>1000248</v>
-      </c>
-      <c r="D249" t="inlineStr"/>
-      <c r="E249" t="inlineStr">
-        <is>
-          <t>Green Public Procurement</t>
-        </is>
-      </c>
-    </row>
-    <row r="250">
-      <c r="A250" s="1" t="n">
-        <v>248</v>
-      </c>
-      <c r="B250" t="n">
-        <v>2000001</v>
-      </c>
-      <c r="C250" t="n">
-        <v>1000249</v>
-      </c>
-      <c r="D250" t="inlineStr"/>
-      <c r="E250" t="inlineStr">
         <is>
           <t>Greening Delle Attività Umane</t>
         </is>

</xml_diff>